<commit_message>
Finished with temporary admin page
</commit_message>
<xml_diff>
--- a/public/excel/beer.xlsx
+++ b/public/excel/beer.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\PhpstormProjects\SmagenAfOl\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\testDir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B397114-DD3A-4230-973E-13A26649E56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81AB3D5-52DF-4E49-9622-B7CC1C55B736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14535" yWindow="510" windowWidth="12150" windowHeight="11385" xr2:uid="{FF801C82-C85B-4F8B-B9B9-9E60977209A2}"/>
+    <workbookView xWindow="-15570" yWindow="8760" windowWidth="12150" windowHeight="7680" xr2:uid="{FF801C82-C85B-4F8B-B9B9-9E60977209A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -55,9 +54,6 @@
     <t>size</t>
   </si>
   <si>
-    <t>filename</t>
-  </si>
-  <si>
     <t>IPA</t>
   </si>
   <si>
@@ -179,6 +175,12 @@
   </si>
   <si>
     <t>Newbarns</t>
+  </si>
+  <si>
+    <t>lemon_drip.jpg</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
 </sst>
 </file>
@@ -532,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C0633C-4057-4AF5-9720-F3BEEDEEB596}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,30 +571,30 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
       <c r="E2">
         <v>6.1</v>
@@ -604,7 +606,7 @@
         <v>440</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -612,16 +614,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
       </c>
       <c r="E3">
         <v>6.5</v>
@@ -633,7 +635,7 @@
         <v>330</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -641,16 +643,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -667,16 +669,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>8.5</v>
@@ -693,16 +695,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
       </c>
       <c r="E6">
         <v>5.5</v>
@@ -713,22 +715,25 @@
       <c r="G6">
         <v>440</v>
       </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
       <c r="I6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -745,16 +750,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
       </c>
       <c r="E8">
         <v>5.7</v>
@@ -766,7 +771,7 @@
         <v>388</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -774,16 +779,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
       <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
       </c>
       <c r="E9">
         <v>12.5</v>
@@ -795,7 +800,7 @@
         <v>330</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -803,16 +808,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
       <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -829,16 +834,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
       </c>
       <c r="E11">
         <v>7</v>
@@ -855,16 +860,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
       </c>
       <c r="E12">
         <v>3</v>

</xml_diff>